<commit_message>
date issue when uploading solved
</commit_message>
<xml_diff>
--- a/shoppingbackend/book1.xlsx
+++ b/shoppingbackend/book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MajorProject\shoppingbackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB599B5-08B1-40F2-8437-CE77F496021C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4A9CD8-737F-4078-8240-395474220842}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3792" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{F001959C-5457-4B5E-9978-A82F543A1465}"/>
+    <workbookView xWindow="0" yWindow="408" windowWidth="11916" windowHeight="8964" xr2:uid="{F001959C-5457-4B5E-9978-A82F543A1465}"/>
   </bookViews>
   <sheets>
     <sheet name="Product_Sample" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -153,8 +153,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27A1A99-2FA3-42AE-8884-E1FCADB6CCC6}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,7 +481,7 @@
     <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>